<commit_message>
Add Jupyter Notebook for WSDP operations with error handling and WS-Security
- Created a new Jupyter Notebook for interacting with the WSDP (Web Services for the Cadastre) API.
- Implemented installation of the required `zeep` library.
- Added code to list available operations and their parameters.
- Included error handling for SOAP faults during API calls.
- Integrated WS-Security for authentication using UsernameToken.
- Provided hard-coded test values for querying property information.
</commit_message>
<xml_diff>
--- a/PYTHON/DATA_ANALYSIS/VALUO/data_strukturovana/___ALL/1/cadastre_report_6_2024 (3).xlsx
+++ b/PYTHON/DATA_ANALYSIS/VALUO/data_strukturovana/___ALL/1/cadastre_report_6_2024 (3).xlsx
@@ -1,21 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3ad31658eb0d26ad/Dokumenty/PROG/PYTHON/DATA_ANALYSIS/VALUO/data_strukturovana/___ALL/1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_85AD53BF65A3DE744003782BDAAEDC2DABF39583" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6D75CE2-9EB2-40B8-B7E1-94533115C155}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="61656" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet!$A$1:$P$282</definedName>
+  </definedNames>
+  <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1056">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3384" uniqueCount="1056">
   <si>
     <t>Číslo vkladu</t>
   </si>
@@ -3188,16 +3209,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00_-"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -3224,14 +3241,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf xfId="0" fontId="0" numFmtId="164" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3521,19 +3546,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:P282"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="J1" sqref="J1:J282"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="20.77734375" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="51" customWidth="1"/>
+    <col min="11" max="11" width="38.44140625" customWidth="1"/>
+    <col min="12" max="12" width="178.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3583,7 +3614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3612,7 +3643,7 @@
         <v>23</v>
       </c>
       <c r="J2" s="1">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
@@ -3633,7 +3664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -3683,7 +3714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -3712,7 +3743,7 @@
         <v>23</v>
       </c>
       <c r="J4" s="1">
-        <v>108.0</v>
+        <v>108</v>
       </c>
       <c r="K4" t="s">
         <v>41</v>
@@ -3733,7 +3764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -3762,7 +3793,7 @@
         <v>23</v>
       </c>
       <c r="J5" s="1">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="K5" t="s">
         <v>41</v>
@@ -3783,7 +3814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -3833,7 +3864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -3883,7 +3914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -3933,7 +3964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -3962,7 +3993,7 @@
         <v>23</v>
       </c>
       <c r="J9" s="1">
-        <v>265.0</v>
+        <v>265</v>
       </c>
       <c r="K9" t="s">
         <v>41</v>
@@ -3983,7 +4014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -4012,7 +4043,7 @@
         <v>23</v>
       </c>
       <c r="J10" s="1">
-        <v>154.0</v>
+        <v>154</v>
       </c>
       <c r="K10" t="s">
         <v>41</v>
@@ -4033,7 +4064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -4062,7 +4093,7 @@
         <v>23</v>
       </c>
       <c r="J11" s="1">
-        <v>265.0</v>
+        <v>265</v>
       </c>
       <c r="K11" t="s">
         <v>41</v>
@@ -4083,7 +4114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -4133,7 +4164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -4183,7 +4214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -4233,7 +4264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -4283,7 +4314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>81</v>
       </c>
@@ -4333,7 +4364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -4362,7 +4393,7 @@
         <v>23</v>
       </c>
       <c r="J17" s="1">
-        <v>464.0</v>
+        <v>464</v>
       </c>
       <c r="K17" t="s">
         <v>41</v>
@@ -4383,7 +4414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>91</v>
       </c>
@@ -4433,7 +4464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>95</v>
       </c>
@@ -4483,7 +4514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -4533,7 +4564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>104</v>
       </c>
@@ -4583,7 +4614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>109</v>
       </c>
@@ -4633,7 +4664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>113</v>
       </c>
@@ -4662,7 +4693,7 @@
         <v>23</v>
       </c>
       <c r="J23" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="K23" t="s">
         <v>41</v>
@@ -4683,7 +4714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>118</v>
       </c>
@@ -4733,7 +4764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>123</v>
       </c>
@@ -4783,7 +4814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -4812,7 +4843,7 @@
         <v>23</v>
       </c>
       <c r="J26" s="1">
-        <v>387.0</v>
+        <v>387</v>
       </c>
       <c r="K26" t="s">
         <v>41</v>
@@ -4833,7 +4864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>128</v>
       </c>
@@ -4862,7 +4893,7 @@
         <v>23</v>
       </c>
       <c r="J27" s="1">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="K27" t="s">
         <v>41</v>
@@ -4883,7 +4914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>135</v>
       </c>
@@ -4912,7 +4943,7 @@
         <v>23</v>
       </c>
       <c r="J28" s="1">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="K28" t="s">
         <v>24</v>
@@ -4933,7 +4964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>140</v>
       </c>
@@ -4983,7 +5014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>144</v>
       </c>
@@ -5033,7 +5064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -5062,7 +5093,7 @@
         <v>23</v>
       </c>
       <c r="J31" s="1">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="K31" t="s">
         <v>24</v>
@@ -5083,7 +5114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>153</v>
       </c>
@@ -5112,7 +5143,7 @@
         <v>23</v>
       </c>
       <c r="J32" s="1">
-        <v>35.62</v>
+        <v>35.619999999999997</v>
       </c>
       <c r="K32" t="s">
         <v>24</v>
@@ -5133,7 +5164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>158</v>
       </c>
@@ -5183,7 +5214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>158</v>
       </c>
@@ -5212,7 +5243,7 @@
         <v>23</v>
       </c>
       <c r="J34" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="K34" t="s">
         <v>41</v>
@@ -5233,7 +5264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>165</v>
       </c>
@@ -5283,7 +5314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>169</v>
       </c>
@@ -5333,7 +5364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>173</v>
       </c>
@@ -5362,7 +5393,7 @@
         <v>23</v>
       </c>
       <c r="J37" s="1">
-        <v>225.0</v>
+        <v>225</v>
       </c>
       <c r="K37" t="s">
         <v>41</v>
@@ -5383,7 +5414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>178</v>
       </c>
@@ -5412,7 +5443,7 @@
         <v>23</v>
       </c>
       <c r="J38" s="1">
-        <v>74.4</v>
+        <v>74.400000000000006</v>
       </c>
       <c r="K38" t="s">
         <v>24</v>
@@ -5433,7 +5464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -5462,7 +5493,7 @@
         <v>23</v>
       </c>
       <c r="J39" s="1">
-        <v>40.37</v>
+        <v>40.369999999999997</v>
       </c>
       <c r="K39" t="s">
         <v>24</v>
@@ -5483,7 +5514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>184</v>
       </c>
@@ -5533,7 +5564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>184</v>
       </c>
@@ -5562,7 +5593,7 @@
         <v>23</v>
       </c>
       <c r="J41" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="K41" t="s">
         <v>41</v>
@@ -5583,7 +5614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>190</v>
       </c>
@@ -5633,7 +5664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>194</v>
       </c>
@@ -5662,7 +5693,7 @@
         <v>23</v>
       </c>
       <c r="J43" s="1">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="K43" t="s">
         <v>24</v>
@@ -5683,7 +5714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>199</v>
       </c>
@@ -5733,7 +5764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>199</v>
       </c>
@@ -5762,7 +5793,7 @@
         <v>23</v>
       </c>
       <c r="J45" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="K45" t="s">
         <v>41</v>
@@ -5783,7 +5814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>205</v>
       </c>
@@ -5833,7 +5864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>205</v>
       </c>
@@ -5862,7 +5893,7 @@
         <v>23</v>
       </c>
       <c r="J47" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="K47" t="s">
         <v>41</v>
@@ -5883,7 +5914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>211</v>
       </c>
@@ -5933,7 +5964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>215</v>
       </c>
@@ -5962,7 +5993,7 @@
         <v>23</v>
       </c>
       <c r="J49" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="K49" t="s">
         <v>41</v>
@@ -5983,7 +6014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>220</v>
       </c>
@@ -6033,7 +6064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>220</v>
       </c>
@@ -6083,7 +6114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>224</v>
       </c>
@@ -6112,7 +6143,7 @@
         <v>23</v>
       </c>
       <c r="J52" s="1">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="K52" t="s">
         <v>24</v>
@@ -6133,7 +6164,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>228</v>
       </c>
@@ -6183,7 +6214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>233</v>
       </c>
@@ -6233,7 +6264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>238</v>
       </c>
@@ -6283,7 +6314,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>242</v>
       </c>
@@ -6333,7 +6364,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>246</v>
       </c>
@@ -6383,7 +6414,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>251</v>
       </c>
@@ -6433,7 +6464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>255</v>
       </c>
@@ -6483,7 +6514,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>255</v>
       </c>
@@ -6512,7 +6543,7 @@
         <v>23</v>
       </c>
       <c r="J60" s="1">
-        <v>15704.0</v>
+        <v>15704</v>
       </c>
       <c r="K60" t="s">
         <v>260</v>
@@ -6533,7 +6564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>255</v>
       </c>
@@ -6562,7 +6593,7 @@
         <v>23</v>
       </c>
       <c r="J61" s="1">
-        <v>149.0</v>
+        <v>149</v>
       </c>
       <c r="K61" t="s">
         <v>41</v>
@@ -6583,7 +6614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>255</v>
       </c>
@@ -6612,7 +6643,7 @@
         <v>23</v>
       </c>
       <c r="J62" s="1">
-        <v>82.0</v>
+        <v>82</v>
       </c>
       <c r="K62" t="s">
         <v>41</v>
@@ -6633,7 +6664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>255</v>
       </c>
@@ -6662,7 +6693,7 @@
         <v>23</v>
       </c>
       <c r="J63" s="1">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="K63" t="s">
         <v>41</v>
@@ -6683,7 +6714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>255</v>
       </c>
@@ -6712,7 +6743,7 @@
         <v>23</v>
       </c>
       <c r="J64" s="1">
-        <v>832.0</v>
+        <v>832</v>
       </c>
       <c r="K64" t="s">
         <v>41</v>
@@ -6733,7 +6764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>255</v>
       </c>
@@ -6762,7 +6793,7 @@
         <v>23</v>
       </c>
       <c r="J65" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="K65" t="s">
         <v>41</v>
@@ -6783,7 +6814,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>273</v>
       </c>
@@ -6833,7 +6864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>277</v>
       </c>
@@ -6862,7 +6893,7 @@
         <v>23</v>
       </c>
       <c r="J67" s="1">
-        <v>263.0</v>
+        <v>263</v>
       </c>
       <c r="K67" t="s">
         <v>41</v>
@@ -6883,7 +6914,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>282</v>
       </c>
@@ -6933,7 +6964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>282</v>
       </c>
@@ -6983,7 +7014,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>288</v>
       </c>
@@ -7012,7 +7043,7 @@
         <v>23</v>
       </c>
       <c r="J70" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="K70" t="s">
         <v>41</v>
@@ -7033,7 +7064,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>288</v>
       </c>
@@ -7062,7 +7093,7 @@
         <v>23</v>
       </c>
       <c r="J71" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="K71" t="s">
         <v>41</v>
@@ -7083,7 +7114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>295</v>
       </c>
@@ -7125,7 +7156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>299</v>
       </c>
@@ -7175,7 +7206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>303</v>
       </c>
@@ -7225,7 +7256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>308</v>
       </c>
@@ -7275,7 +7306,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>308</v>
       </c>
@@ -7325,7 +7356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>312</v>
       </c>
@@ -7354,7 +7385,7 @@
         <v>23</v>
       </c>
       <c r="J77" s="1">
-        <v>64.4</v>
+        <v>64.400000000000006</v>
       </c>
       <c r="K77" t="s">
         <v>24</v>
@@ -7375,7 +7406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>316</v>
       </c>
@@ -7425,7 +7456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>316</v>
       </c>
@@ -7454,7 +7485,7 @@
         <v>23</v>
       </c>
       <c r="J79" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="K79" t="s">
         <v>41</v>
@@ -7475,7 +7506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>322</v>
       </c>
@@ -7525,7 +7556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>322</v>
       </c>
@@ -7575,7 +7606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>326</v>
       </c>
@@ -7625,7 +7656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>326</v>
       </c>
@@ -7654,7 +7685,7 @@
         <v>23</v>
       </c>
       <c r="J83" s="1">
-        <v>208.0</v>
+        <v>208</v>
       </c>
       <c r="K83" t="s">
         <v>41</v>
@@ -7675,7 +7706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>326</v>
       </c>
@@ -7704,7 +7735,7 @@
         <v>23</v>
       </c>
       <c r="J84" s="1">
-        <v>184.0</v>
+        <v>184</v>
       </c>
       <c r="K84" t="s">
         <v>41</v>
@@ -7725,7 +7756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>335</v>
       </c>
@@ -7754,7 +7785,7 @@
         <v>23</v>
       </c>
       <c r="J85" s="1">
-        <v>157.0</v>
+        <v>157</v>
       </c>
       <c r="K85" t="s">
         <v>41</v>
@@ -7775,7 +7806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>340</v>
       </c>
@@ -7825,7 +7856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>344</v>
       </c>
@@ -7854,7 +7885,7 @@
         <v>23</v>
       </c>
       <c r="J87" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="K87" t="s">
         <v>41</v>
@@ -7875,7 +7906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>349</v>
       </c>
@@ -7925,7 +7956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>354</v>
       </c>
@@ -7975,7 +8006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>358</v>
       </c>
@@ -8025,7 +8056,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>363</v>
       </c>
@@ -8075,7 +8106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>367</v>
       </c>
@@ -8104,7 +8135,7 @@
         <v>23</v>
       </c>
       <c r="J92" s="1">
-        <v>182.0</v>
+        <v>182</v>
       </c>
       <c r="K92" t="s">
         <v>41</v>
@@ -8125,7 +8156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>372</v>
       </c>
@@ -8175,7 +8206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>376</v>
       </c>
@@ -8204,7 +8235,7 @@
         <v>23</v>
       </c>
       <c r="J94" s="1">
-        <v>2407.0</v>
+        <v>2407</v>
       </c>
       <c r="K94" t="s">
         <v>41</v>
@@ -8225,7 +8256,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>376</v>
       </c>
@@ -8254,7 +8285,7 @@
         <v>23</v>
       </c>
       <c r="J95" s="1">
-        <v>18318.0</v>
+        <v>18318</v>
       </c>
       <c r="K95" t="s">
         <v>41</v>
@@ -8275,7 +8306,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>384</v>
       </c>
@@ -8304,7 +8335,7 @@
         <v>23</v>
       </c>
       <c r="J96" s="1">
-        <v>276.0</v>
+        <v>276</v>
       </c>
       <c r="K96" t="s">
         <v>41</v>
@@ -8325,7 +8356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>384</v>
       </c>
@@ -8354,7 +8385,7 @@
         <v>23</v>
       </c>
       <c r="J97" s="1">
-        <v>253.0</v>
+        <v>253</v>
       </c>
       <c r="K97" t="s">
         <v>41</v>
@@ -8375,7 +8406,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>391</v>
       </c>
@@ -8425,7 +8456,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>396</v>
       </c>
@@ -8475,7 +8506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>400</v>
       </c>
@@ -8525,7 +8556,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>404</v>
       </c>
@@ -8575,7 +8606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>408</v>
       </c>
@@ -8604,7 +8635,7 @@
         <v>23</v>
       </c>
       <c r="J102" s="1">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="K102" t="s">
         <v>24</v>
@@ -8625,7 +8656,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>413</v>
       </c>
@@ -8654,7 +8685,7 @@
         <v>23</v>
       </c>
       <c r="J103" s="1">
-        <v>256.0</v>
+        <v>256</v>
       </c>
       <c r="K103" t="s">
         <v>41</v>
@@ -8675,7 +8706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>419</v>
       </c>
@@ -8725,7 +8756,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>419</v>
       </c>
@@ -8754,7 +8785,7 @@
         <v>23</v>
       </c>
       <c r="J105" s="1">
-        <v>88.0</v>
+        <v>88</v>
       </c>
       <c r="K105" t="s">
         <v>41</v>
@@ -8775,7 +8806,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>427</v>
       </c>
@@ -8825,7 +8856,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>432</v>
       </c>
@@ -8875,7 +8906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>436</v>
       </c>
@@ -8904,7 +8935,7 @@
         <v>23</v>
       </c>
       <c r="J108" s="1">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="K108" t="s">
         <v>24</v>
@@ -8925,7 +8956,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>440</v>
       </c>
@@ -8975,7 +9006,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>444</v>
       </c>
@@ -9004,7 +9035,7 @@
         <v>23</v>
       </c>
       <c r="J110" s="1">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="K110" t="s">
         <v>41</v>
@@ -9025,7 +9056,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>449</v>
       </c>
@@ -9075,7 +9106,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>454</v>
       </c>
@@ -9104,7 +9135,7 @@
         <v>23</v>
       </c>
       <c r="J112" s="1">
-        <v>80.1</v>
+        <v>80.099999999999994</v>
       </c>
       <c r="K112" t="s">
         <v>24</v>
@@ -9125,7 +9156,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>454</v>
       </c>
@@ -9154,7 +9185,7 @@
         <v>23</v>
       </c>
       <c r="J113" s="1">
-        <v>375.0</v>
+        <v>375</v>
       </c>
       <c r="K113" t="s">
         <v>41</v>
@@ -9175,7 +9206,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>460</v>
       </c>
@@ -9217,7 +9248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>464</v>
       </c>
@@ -9246,7 +9277,7 @@
         <v>23</v>
       </c>
       <c r="J115" s="1">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="K115" t="s">
         <v>24</v>
@@ -9267,7 +9298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>464</v>
       </c>
@@ -9296,7 +9327,7 @@
         <v>23</v>
       </c>
       <c r="J116" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="K116" t="s">
         <v>41</v>
@@ -9317,7 +9348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>470</v>
       </c>
@@ -9367,7 +9398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>474</v>
       </c>
@@ -9417,7 +9448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>479</v>
       </c>
@@ -9446,7 +9477,7 @@
         <v>23</v>
       </c>
       <c r="J119" s="1">
-        <v>254.0</v>
+        <v>254</v>
       </c>
       <c r="K119" t="s">
         <v>41</v>
@@ -9467,7 +9498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>479</v>
       </c>
@@ -9496,7 +9527,7 @@
         <v>23</v>
       </c>
       <c r="J120" s="1">
-        <v>329.0</v>
+        <v>329</v>
       </c>
       <c r="K120" t="s">
         <v>41</v>
@@ -9517,7 +9548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>486</v>
       </c>
@@ -9567,7 +9598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>490</v>
       </c>
@@ -9617,7 +9648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>493</v>
       </c>
@@ -9646,7 +9677,7 @@
         <v>23</v>
       </c>
       <c r="J123" s="1">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="K123" t="s">
         <v>41</v>
@@ -9667,7 +9698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>499</v>
       </c>
@@ -9717,7 +9748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>504</v>
       </c>
@@ -9746,7 +9777,7 @@
         <v>23</v>
       </c>
       <c r="J125" s="1">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="K125" t="s">
         <v>24</v>
@@ -9767,7 +9798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>509</v>
       </c>
@@ -9817,7 +9848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>513</v>
       </c>
@@ -9867,7 +9898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>517</v>
       </c>
@@ -9917,7 +9948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>517</v>
       </c>
@@ -9967,7 +9998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="130" spans="1:16">
+    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>517</v>
       </c>
@@ -10017,7 +10048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="131" spans="1:16">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>522</v>
       </c>
@@ -10067,7 +10098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="1:16">
+    <row r="132" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>526</v>
       </c>
@@ -10117,7 +10148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:16">
+    <row r="133" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>526</v>
       </c>
@@ -10146,7 +10177,7 @@
         <v>23</v>
       </c>
       <c r="J133" s="1">
-        <v>132.0</v>
+        <v>132</v>
       </c>
       <c r="K133" t="s">
         <v>41</v>
@@ -10167,7 +10198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="134" spans="1:16">
+    <row r="134" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>526</v>
       </c>
@@ -10196,7 +10227,7 @@
         <v>23</v>
       </c>
       <c r="J134" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="K134" t="s">
         <v>41</v>
@@ -10217,7 +10248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:16">
+    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>526</v>
       </c>
@@ -10246,7 +10277,7 @@
         <v>23</v>
       </c>
       <c r="J135" s="1">
-        <v>229.0</v>
+        <v>229</v>
       </c>
       <c r="K135" t="s">
         <v>41</v>
@@ -10267,7 +10298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="136" spans="1:16">
+    <row r="136" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>526</v>
       </c>
@@ -10296,7 +10327,7 @@
         <v>23</v>
       </c>
       <c r="J136" s="1">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="K136" t="s">
         <v>41</v>
@@ -10317,7 +10348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:16">
+    <row r="137" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>526</v>
       </c>
@@ -10346,7 +10377,7 @@
         <v>23</v>
       </c>
       <c r="J137" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="K137" t="s">
         <v>41</v>
@@ -10367,7 +10398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="138" spans="1:16">
+    <row r="138" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>526</v>
       </c>
@@ -10396,7 +10427,7 @@
         <v>23</v>
       </c>
       <c r="J138" s="1">
-        <v>91.0</v>
+        <v>91</v>
       </c>
       <c r="K138" t="s">
         <v>41</v>
@@ -10417,7 +10448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="139" spans="1:16">
+    <row r="139" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>526</v>
       </c>
@@ -10446,7 +10477,7 @@
         <v>23</v>
       </c>
       <c r="J139" s="1">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="K139" t="s">
         <v>41</v>
@@ -10467,7 +10498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="140" spans="1:16">
+    <row r="140" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>526</v>
       </c>
@@ -10496,7 +10527,7 @@
         <v>23</v>
       </c>
       <c r="J140" s="1">
-        <v>308.0</v>
+        <v>308</v>
       </c>
       <c r="K140" t="s">
         <v>41</v>
@@ -10517,7 +10548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="141" spans="1:16">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>548</v>
       </c>
@@ -10567,7 +10598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:16">
+    <row r="142" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>552</v>
       </c>
@@ -10596,7 +10627,7 @@
         <v>23</v>
       </c>
       <c r="J142" s="1">
-        <v>211.0</v>
+        <v>211</v>
       </c>
       <c r="K142" t="s">
         <v>41</v>
@@ -10617,7 +10648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:16">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>558</v>
       </c>
@@ -10667,7 +10698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="144" spans="1:16">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>562</v>
       </c>
@@ -10717,7 +10748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="145" spans="1:16">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>566</v>
       </c>
@@ -10767,7 +10798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="146" spans="1:16">
+    <row r="146" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>570</v>
       </c>
@@ -10796,7 +10827,7 @@
         <v>23</v>
       </c>
       <c r="J146" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="K146" t="s">
         <v>41</v>
@@ -10817,7 +10848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="147" spans="1:16">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>575</v>
       </c>
@@ -10867,7 +10898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:16">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>579</v>
       </c>
@@ -10917,7 +10948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="149" spans="1:16">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>583</v>
       </c>
@@ -10967,7 +10998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="150" spans="1:16">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>587</v>
       </c>
@@ -10996,7 +11027,7 @@
         <v>23</v>
       </c>
       <c r="J150" s="1">
-        <v>75.4</v>
+        <v>75.400000000000006</v>
       </c>
       <c r="K150" t="s">
         <v>24</v>
@@ -11017,7 +11048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="151" spans="1:16">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>591</v>
       </c>
@@ -11067,7 +11098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="1:16">
+    <row r="152" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>595</v>
       </c>
@@ -11096,7 +11127,7 @@
         <v>23</v>
       </c>
       <c r="J152" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="K152" t="s">
         <v>41</v>
@@ -11117,7 +11148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="153" spans="1:16">
+    <row r="153" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>595</v>
       </c>
@@ -11146,7 +11177,7 @@
         <v>23</v>
       </c>
       <c r="J153" s="1">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="K153" t="s">
         <v>41</v>
@@ -11167,7 +11198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="154" spans="1:16">
+    <row r="154" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>595</v>
       </c>
@@ -11196,7 +11227,7 @@
         <v>23</v>
       </c>
       <c r="J154" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="K154" t="s">
         <v>41</v>
@@ -11217,7 +11248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="155" spans="1:16">
+    <row r="155" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>604</v>
       </c>
@@ -11246,7 +11277,7 @@
         <v>23</v>
       </c>
       <c r="J155" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K155" t="s">
         <v>41</v>
@@ -11267,7 +11298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:16">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>609</v>
       </c>
@@ -11296,7 +11327,7 @@
         <v>23</v>
       </c>
       <c r="J156" s="1">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="K156" t="s">
         <v>24</v>
@@ -11317,7 +11348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="157" spans="1:16">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>614</v>
       </c>
@@ -11367,7 +11398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:16">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>618</v>
       </c>
@@ -11417,7 +11448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="1:16">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>622</v>
       </c>
@@ -11467,7 +11498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="160" spans="1:16">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>626</v>
       </c>
@@ -11517,7 +11548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:16">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>630</v>
       </c>
@@ -11567,7 +11598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:16">
+    <row r="162" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>630</v>
       </c>
@@ -11596,7 +11627,7 @@
         <v>23</v>
       </c>
       <c r="J162" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="K162" t="s">
         <v>41</v>
@@ -11617,7 +11648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="1:16">
+    <row r="163" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>630</v>
       </c>
@@ -11646,7 +11677,7 @@
         <v>23</v>
       </c>
       <c r="J163" s="1">
-        <v>1181.0</v>
+        <v>1181</v>
       </c>
       <c r="K163" t="s">
         <v>41</v>
@@ -11667,7 +11698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:16">
+    <row r="164" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>630</v>
       </c>
@@ -11696,7 +11727,7 @@
         <v>23</v>
       </c>
       <c r="J164" s="1">
-        <v>525.0</v>
+        <v>525</v>
       </c>
       <c r="K164" t="s">
         <v>41</v>
@@ -11717,7 +11748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="165" spans="1:16">
+    <row r="165" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>630</v>
       </c>
@@ -11746,7 +11777,7 @@
         <v>23</v>
       </c>
       <c r="J165" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="K165" t="s">
         <v>41</v>
@@ -11767,7 +11798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="166" spans="1:16">
+    <row r="166" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>643</v>
       </c>
@@ -11796,7 +11827,7 @@
         <v>23</v>
       </c>
       <c r="J166" s="1">
-        <v>12914.0</v>
+        <v>12914</v>
       </c>
       <c r="K166" t="s">
         <v>41</v>
@@ -11817,7 +11848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="167" spans="1:16">
+    <row r="167" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>643</v>
       </c>
@@ -11846,7 +11877,7 @@
         <v>23</v>
       </c>
       <c r="J167" s="1">
-        <v>2758.0</v>
+        <v>2758</v>
       </c>
       <c r="K167" t="s">
         <v>41</v>
@@ -11867,7 +11898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="1:16">
+    <row r="168" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>643</v>
       </c>
@@ -11896,7 +11927,7 @@
         <v>23</v>
       </c>
       <c r="J168" s="1">
-        <v>12366.0</v>
+        <v>12366</v>
       </c>
       <c r="K168" t="s">
         <v>41</v>
@@ -11917,7 +11948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="169" spans="1:16">
+    <row r="169" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>643</v>
       </c>
@@ -11946,7 +11977,7 @@
         <v>23</v>
       </c>
       <c r="J169" s="1">
-        <v>192.0</v>
+        <v>192</v>
       </c>
       <c r="K169" t="s">
         <v>41</v>
@@ -11967,7 +11998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="170" spans="1:16">
+    <row r="170" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>643</v>
       </c>
@@ -11996,7 +12027,7 @@
         <v>23</v>
       </c>
       <c r="J170" s="1">
-        <v>7166.0</v>
+        <v>7166</v>
       </c>
       <c r="K170" t="s">
         <v>41</v>
@@ -12017,7 +12048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="1:16">
+    <row r="171" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>643</v>
       </c>
@@ -12046,7 +12077,7 @@
         <v>23</v>
       </c>
       <c r="J171" s="1">
-        <v>10238.0</v>
+        <v>10238</v>
       </c>
       <c r="K171" t="s">
         <v>41</v>
@@ -12067,7 +12098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="172" spans="1:16">
+    <row r="172" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>643</v>
       </c>
@@ -12096,7 +12127,7 @@
         <v>23</v>
       </c>
       <c r="J172" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="K172" t="s">
         <v>41</v>
@@ -12117,7 +12148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="173" spans="1:16">
+    <row r="173" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>643</v>
       </c>
@@ -12146,7 +12177,7 @@
         <v>23</v>
       </c>
       <c r="J173" s="1">
-        <v>429.0</v>
+        <v>429</v>
       </c>
       <c r="K173" t="s">
         <v>41</v>
@@ -12167,7 +12198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="174" spans="1:16">
+    <row r="174" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>643</v>
       </c>
@@ -12196,7 +12227,7 @@
         <v>23</v>
       </c>
       <c r="J174" s="1">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="K174" t="s">
         <v>41</v>
@@ -12217,7 +12248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="175" spans="1:16">
+    <row r="175" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>643</v>
       </c>
@@ -12246,7 +12277,7 @@
         <v>23</v>
       </c>
       <c r="J175" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="K175" t="s">
         <v>41</v>
@@ -12267,7 +12298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:16">
+    <row r="176" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>643</v>
       </c>
@@ -12296,7 +12327,7 @@
         <v>23</v>
       </c>
       <c r="J176" s="1">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="K176" t="s">
         <v>41</v>
@@ -12317,7 +12348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="177" spans="1:16">
+    <row r="177" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>669</v>
       </c>
@@ -12346,7 +12377,7 @@
         <v>23</v>
       </c>
       <c r="J177" s="1">
-        <v>430.0</v>
+        <v>430</v>
       </c>
       <c r="K177" t="s">
         <v>41</v>
@@ -12367,7 +12398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="178" spans="1:16">
+    <row r="178" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>674</v>
       </c>
@@ -12417,7 +12448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="179" spans="1:16">
+    <row r="179" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>679</v>
       </c>
@@ -12446,7 +12477,7 @@
         <v>23</v>
       </c>
       <c r="J179" s="1">
-        <v>118.0</v>
+        <v>118</v>
       </c>
       <c r="K179" t="s">
         <v>41</v>
@@ -12467,7 +12498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:16">
+    <row r="180" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>684</v>
       </c>
@@ -12496,7 +12527,7 @@
         <v>23</v>
       </c>
       <c r="J180" s="1">
-        <v>518.0</v>
+        <v>518</v>
       </c>
       <c r="K180" t="s">
         <v>41</v>
@@ -12517,7 +12548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="181" spans="1:16">
+    <row r="181" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>684</v>
       </c>
@@ -12546,7 +12577,7 @@
         <v>23</v>
       </c>
       <c r="J181" s="1">
-        <v>305.0</v>
+        <v>305</v>
       </c>
       <c r="K181" t="s">
         <v>41</v>
@@ -12567,7 +12598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:16">
+    <row r="182" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>684</v>
       </c>
@@ -12596,7 +12627,7 @@
         <v>23</v>
       </c>
       <c r="J182" s="1">
-        <v>1289.0</v>
+        <v>1289</v>
       </c>
       <c r="K182" t="s">
         <v>41</v>
@@ -12617,7 +12648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="183" spans="1:16">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>694</v>
       </c>
@@ -12667,7 +12698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="184" spans="1:16">
+    <row r="184" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>694</v>
       </c>
@@ -12696,7 +12727,7 @@
         <v>23</v>
       </c>
       <c r="J184" s="1">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="K184" t="s">
         <v>41</v>
@@ -12717,7 +12748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="185" spans="1:16">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>701</v>
       </c>
@@ -12767,7 +12798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="186" spans="1:16">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>705</v>
       </c>
@@ -12817,7 +12848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:16">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>710</v>
       </c>
@@ -12846,7 +12877,7 @@
         <v>23</v>
       </c>
       <c r="J187" s="1">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="K187" t="s">
         <v>24</v>
@@ -12867,7 +12898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="188" spans="1:16">
+    <row r="188" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>710</v>
       </c>
@@ -12896,7 +12927,7 @@
         <v>23</v>
       </c>
       <c r="J188" s="1">
-        <v>213.0</v>
+        <v>213</v>
       </c>
       <c r="K188" t="s">
         <v>41</v>
@@ -12917,7 +12948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="189" spans="1:16">
+    <row r="189" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>710</v>
       </c>
@@ -12946,7 +12977,7 @@
         <v>23</v>
       </c>
       <c r="J189" s="1">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="K189" t="s">
         <v>41</v>
@@ -12967,7 +12998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="190" spans="1:16">
+    <row r="190" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>710</v>
       </c>
@@ -12996,7 +13027,7 @@
         <v>23</v>
       </c>
       <c r="J190" s="1">
-        <v>207.0</v>
+        <v>207</v>
       </c>
       <c r="K190" t="s">
         <v>41</v>
@@ -13017,7 +13048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="191" spans="1:16">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>720</v>
       </c>
@@ -13046,7 +13077,7 @@
         <v>23</v>
       </c>
       <c r="J191" s="1">
-        <v>78.6</v>
+        <v>78.599999999999994</v>
       </c>
       <c r="K191" t="s">
         <v>24</v>
@@ -13067,7 +13098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="192" spans="1:16">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>725</v>
       </c>
@@ -13117,7 +13148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="193" spans="1:16">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>729</v>
       </c>
@@ -13146,7 +13177,7 @@
         <v>23</v>
       </c>
       <c r="J193" s="1">
-        <v>232.0</v>
+        <v>232</v>
       </c>
       <c r="K193" t="s">
         <v>41</v>
@@ -13167,7 +13198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="194" spans="1:16">
+    <row r="194" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>729</v>
       </c>
@@ -13196,7 +13227,7 @@
         <v>23</v>
       </c>
       <c r="J194" s="1">
-        <v>232.0</v>
+        <v>232</v>
       </c>
       <c r="K194" t="s">
         <v>41</v>
@@ -13217,7 +13248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="195" spans="1:16">
+    <row r="195" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>729</v>
       </c>
@@ -13246,7 +13277,7 @@
         <v>23</v>
       </c>
       <c r="J195" s="1">
-        <v>223.0</v>
+        <v>223</v>
       </c>
       <c r="K195" t="s">
         <v>41</v>
@@ -13267,7 +13298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="196" spans="1:16">
+    <row r="196" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>737</v>
       </c>
@@ -13296,7 +13327,7 @@
         <v>23</v>
       </c>
       <c r="J196" s="1">
-        <v>614.0</v>
+        <v>614</v>
       </c>
       <c r="K196" t="s">
         <v>41</v>
@@ -13317,7 +13348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:16">
+    <row r="197" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>737</v>
       </c>
@@ -13346,7 +13377,7 @@
         <v>23</v>
       </c>
       <c r="J197" s="1">
-        <v>1988.0</v>
+        <v>1988</v>
       </c>
       <c r="K197" t="s">
         <v>41</v>
@@ -13367,7 +13398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="198" spans="1:16">
+    <row r="198" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>737</v>
       </c>
@@ -13396,7 +13427,7 @@
         <v>23</v>
       </c>
       <c r="J198" s="1">
-        <v>352.0</v>
+        <v>352</v>
       </c>
       <c r="K198" t="s">
         <v>41</v>
@@ -13417,7 +13448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="199" spans="1:16">
+    <row r="199" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>737</v>
       </c>
@@ -13446,7 +13477,7 @@
         <v>23</v>
       </c>
       <c r="J199" s="1">
-        <v>207.0</v>
+        <v>207</v>
       </c>
       <c r="K199" t="s">
         <v>41</v>
@@ -13467,7 +13498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="200" spans="1:16">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>749</v>
       </c>
@@ -13517,7 +13548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="201" spans="1:16">
+    <row r="201" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>753</v>
       </c>
@@ -13546,7 +13577,7 @@
         <v>23</v>
       </c>
       <c r="J201" s="1">
-        <v>583.0</v>
+        <v>583</v>
       </c>
       <c r="K201" t="s">
         <v>41</v>
@@ -13567,7 +13598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="202" spans="1:16">
+    <row r="202" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>753</v>
       </c>
@@ -13596,7 +13627,7 @@
         <v>23</v>
       </c>
       <c r="J202" s="1">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="K202" t="s">
         <v>41</v>
@@ -13617,7 +13648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="203" spans="1:16">
+    <row r="203" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>753</v>
       </c>
@@ -13646,7 +13677,7 @@
         <v>23</v>
       </c>
       <c r="J203" s="1">
-        <v>105.0</v>
+        <v>105</v>
       </c>
       <c r="K203" t="s">
         <v>41</v>
@@ -13667,7 +13698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="204" spans="1:16">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>760</v>
       </c>
@@ -13696,7 +13727,7 @@
         <v>23</v>
       </c>
       <c r="J204" s="1">
-        <v>226.0</v>
+        <v>226</v>
       </c>
       <c r="K204" t="s">
         <v>41</v>
@@ -13717,7 +13748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="205" spans="1:16">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>765</v>
       </c>
@@ -13767,7 +13798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="206" spans="1:16">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>769</v>
       </c>
@@ -13817,7 +13848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="207" spans="1:16">
+    <row r="207" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>769</v>
       </c>
@@ -13846,7 +13877,7 @@
         <v>23</v>
       </c>
       <c r="J207" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="K207" t="s">
         <v>41</v>
@@ -13867,7 +13898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="208" spans="1:16">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>775</v>
       </c>
@@ -13896,7 +13927,7 @@
         <v>23</v>
       </c>
       <c r="J208" s="1">
-        <v>36.3</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="K208" t="s">
         <v>24</v>
@@ -13917,7 +13948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="209" spans="1:16">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>780</v>
       </c>
@@ -13967,7 +13998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="210" spans="1:16">
+    <row r="210" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>784</v>
       </c>
@@ -13996,7 +14027,7 @@
         <v>23</v>
       </c>
       <c r="J210" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="K210" t="s">
         <v>41</v>
@@ -14017,7 +14048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="211" spans="1:16">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>789</v>
       </c>
@@ -14067,7 +14098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:16">
+    <row r="212" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>793</v>
       </c>
@@ -14096,7 +14127,7 @@
         <v>23</v>
       </c>
       <c r="J212" s="1">
-        <v>286.0</v>
+        <v>286</v>
       </c>
       <c r="K212" t="s">
         <v>41</v>
@@ -14117,7 +14148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="213" spans="1:16">
+    <row r="213" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>793</v>
       </c>
@@ -14146,7 +14177,7 @@
         <v>23</v>
       </c>
       <c r="J213" s="1">
-        <v>81.0</v>
+        <v>81</v>
       </c>
       <c r="K213" t="s">
         <v>41</v>
@@ -14167,7 +14198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="214" spans="1:16">
+    <row r="214" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>793</v>
       </c>
@@ -14196,7 +14227,7 @@
         <v>23</v>
       </c>
       <c r="J214" s="1">
-        <v>210.0</v>
+        <v>210</v>
       </c>
       <c r="K214" t="s">
         <v>41</v>
@@ -14217,7 +14248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="215" spans="1:16">
+    <row r="215" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>793</v>
       </c>
@@ -14246,7 +14277,7 @@
         <v>23</v>
       </c>
       <c r="J215" s="1">
-        <v>175.0</v>
+        <v>175</v>
       </c>
       <c r="K215" t="s">
         <v>41</v>
@@ -14267,7 +14298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="216" spans="1:16">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>806</v>
       </c>
@@ -14317,7 +14348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="217" spans="1:16">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>810</v>
       </c>
@@ -14346,7 +14377,7 @@
         <v>23</v>
       </c>
       <c r="J217" s="1">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="K217" t="s">
         <v>24</v>
@@ -14367,7 +14398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="218" spans="1:16">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>815</v>
       </c>
@@ -14396,7 +14427,7 @@
         <v>23</v>
       </c>
       <c r="J218" s="1">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="K218" t="s">
         <v>24</v>
@@ -14417,7 +14448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="219" spans="1:16">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>815</v>
       </c>
@@ -14467,7 +14498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="220" spans="1:16">
+    <row r="220" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>815</v>
       </c>
@@ -14517,7 +14548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="221" spans="1:16">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>820</v>
       </c>
@@ -14546,7 +14577,7 @@
         <v>23</v>
       </c>
       <c r="J221" s="1">
-        <v>220.0</v>
+        <v>220</v>
       </c>
       <c r="K221" t="s">
         <v>41</v>
@@ -14567,7 +14598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="222" spans="1:16">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>825</v>
       </c>
@@ -14617,7 +14648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="223" spans="1:16">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>829</v>
       </c>
@@ -14667,7 +14698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="224" spans="1:16">
+    <row r="224" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>833</v>
       </c>
@@ -14696,7 +14727,7 @@
         <v>23</v>
       </c>
       <c r="J224" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="K224" t="s">
         <v>41</v>
@@ -14717,7 +14748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="225" spans="1:16">
+    <row r="225" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>838</v>
       </c>
@@ -14767,7 +14798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="226" spans="1:16">
+    <row r="226" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>842</v>
       </c>
@@ -14796,7 +14827,7 @@
         <v>23</v>
       </c>
       <c r="J226" s="1">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="K226" t="s">
         <v>24</v>
@@ -14817,7 +14848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="227" spans="1:16">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>847</v>
       </c>
@@ -14867,7 +14898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="228" spans="1:16">
+    <row r="228" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>851</v>
       </c>
@@ -14917,7 +14948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="229" spans="1:16">
+    <row r="229" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>855</v>
       </c>
@@ -14946,7 +14977,7 @@
         <v>23</v>
       </c>
       <c r="J229" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="K229" t="s">
         <v>41</v>
@@ -14967,7 +14998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="230" spans="1:16">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>860</v>
       </c>
@@ -15017,7 +15048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="231" spans="1:16">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>864</v>
       </c>
@@ -15067,7 +15098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="232" spans="1:16">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>868</v>
       </c>
@@ -15117,7 +15148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="233" spans="1:16">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>872</v>
       </c>
@@ -15167,7 +15198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="234" spans="1:16">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>876</v>
       </c>
@@ -15217,7 +15248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="235" spans="1:16">
+    <row r="235" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>876</v>
       </c>
@@ -15246,7 +15277,7 @@
         <v>23</v>
       </c>
       <c r="J235" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="K235" t="s">
         <v>41</v>
@@ -15267,7 +15298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="236" spans="1:16">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>882</v>
       </c>
@@ -15317,7 +15348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="237" spans="1:16">
+    <row r="237" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>887</v>
       </c>
@@ -15346,7 +15377,7 @@
         <v>23</v>
       </c>
       <c r="J237" s="1">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="K237" t="s">
         <v>24</v>
@@ -15367,7 +15398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="238" spans="1:16">
+    <row r="238" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>887</v>
       </c>
@@ -15417,7 +15448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="239" spans="1:16">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>891</v>
       </c>
@@ -15467,7 +15498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="240" spans="1:16">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>896</v>
       </c>
@@ -15496,7 +15527,7 @@
         <v>23</v>
       </c>
       <c r="J240" s="1">
-        <v>71.4</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="K240" t="s">
         <v>24</v>
@@ -15517,7 +15548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="241" spans="1:16">
+    <row r="241" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>900</v>
       </c>
@@ -15567,7 +15598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="242" spans="1:16">
+    <row r="242" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>905</v>
       </c>
@@ -15596,7 +15627,7 @@
         <v>23</v>
       </c>
       <c r="J242" s="1">
-        <v>113.0</v>
+        <v>113</v>
       </c>
       <c r="K242" t="s">
         <v>260</v>
@@ -15617,7 +15648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="243" spans="1:16">
+    <row r="243" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>905</v>
       </c>
@@ -15646,7 +15677,7 @@
         <v>23</v>
       </c>
       <c r="J243" s="1">
-        <v>236.0</v>
+        <v>236</v>
       </c>
       <c r="K243" t="s">
         <v>41</v>
@@ -15667,7 +15698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="244" spans="1:16">
+    <row r="244" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>912</v>
       </c>
@@ -15696,7 +15727,7 @@
         <v>23</v>
       </c>
       <c r="J244" s="1">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="K244" t="s">
         <v>41</v>
@@ -15717,7 +15748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:16">
+    <row r="245" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>912</v>
       </c>
@@ -15746,7 +15777,7 @@
         <v>23</v>
       </c>
       <c r="J245" s="1">
-        <v>91.0</v>
+        <v>91</v>
       </c>
       <c r="K245" t="s">
         <v>41</v>
@@ -15767,7 +15798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="246" spans="1:16">
+    <row r="246" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>919</v>
       </c>
@@ -15817,7 +15848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="247" spans="1:16">
+    <row r="247" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>923</v>
       </c>
@@ -15867,7 +15898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="248" spans="1:16">
+    <row r="248" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>927</v>
       </c>
@@ -15917,7 +15948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="249" spans="1:16">
+    <row r="249" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>931</v>
       </c>
@@ -15946,7 +15977,7 @@
         <v>23</v>
       </c>
       <c r="J249" s="1">
-        <v>392.0</v>
+        <v>392</v>
       </c>
       <c r="K249" t="s">
         <v>41</v>
@@ -15967,7 +15998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="250" spans="1:16">
+    <row r="250" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>936</v>
       </c>
@@ -15996,7 +16027,7 @@
         <v>23</v>
       </c>
       <c r="J250" s="1">
-        <v>119.0</v>
+        <v>119</v>
       </c>
       <c r="K250" t="s">
         <v>41</v>
@@ -16017,7 +16048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="251" spans="1:16">
+    <row r="251" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>936</v>
       </c>
@@ -16046,7 +16077,7 @@
         <v>23</v>
       </c>
       <c r="J251" s="1">
-        <v>620.0</v>
+        <v>620</v>
       </c>
       <c r="K251" t="s">
         <v>41</v>
@@ -16067,7 +16098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="252" spans="1:16">
+    <row r="252" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>943</v>
       </c>
@@ -16096,7 +16127,7 @@
         <v>23</v>
       </c>
       <c r="J252" s="1">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="K252" t="s">
         <v>24</v>
@@ -16117,7 +16148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="253" spans="1:16">
+    <row r="253" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>948</v>
       </c>
@@ -16146,7 +16177,7 @@
         <v>23</v>
       </c>
       <c r="J253" s="1">
-        <v>126.0</v>
+        <v>126</v>
       </c>
       <c r="K253" t="s">
         <v>41</v>
@@ -16167,7 +16198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="254" spans="1:16">
+    <row r="254" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>948</v>
       </c>
@@ -16196,7 +16227,7 @@
         <v>23</v>
       </c>
       <c r="J254" s="1">
-        <v>161.0</v>
+        <v>161</v>
       </c>
       <c r="K254" t="s">
         <v>41</v>
@@ -16217,7 +16248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="255" spans="1:16">
+    <row r="255" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>955</v>
       </c>
@@ -16267,7 +16298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="256" spans="1:16">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>960</v>
       </c>
@@ -16296,7 +16327,7 @@
         <v>23</v>
       </c>
       <c r="J256" s="1">
-        <v>231.0</v>
+        <v>231</v>
       </c>
       <c r="K256" t="s">
         <v>41</v>
@@ -16317,7 +16348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="257" spans="1:16">
+    <row r="257" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>965</v>
       </c>
@@ -16346,7 +16377,7 @@
         <v>23</v>
       </c>
       <c r="J257" s="1">
-        <v>256.0</v>
+        <v>256</v>
       </c>
       <c r="K257" t="s">
         <v>41</v>
@@ -16367,7 +16398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="258" spans="1:16">
+    <row r="258" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>968</v>
       </c>
@@ -16396,7 +16427,7 @@
         <v>23</v>
       </c>
       <c r="J258" s="1">
-        <v>176.0</v>
+        <v>176</v>
       </c>
       <c r="K258" t="s">
         <v>41</v>
@@ -16417,7 +16448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="259" spans="1:16">
+    <row r="259" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>973</v>
       </c>
@@ -16446,7 +16477,7 @@
         <v>23</v>
       </c>
       <c r="J259" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="K259" t="s">
         <v>41</v>
@@ -16467,7 +16498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="260" spans="1:16">
+    <row r="260" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>978</v>
       </c>
@@ -16517,7 +16548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="261" spans="1:16">
+    <row r="261" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>983</v>
       </c>
@@ -16546,7 +16577,7 @@
         <v>23</v>
       </c>
       <c r="J261" s="1">
-        <v>75.4</v>
+        <v>75.400000000000006</v>
       </c>
       <c r="K261" t="s">
         <v>24</v>
@@ -16567,7 +16598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="262" spans="1:16">
+    <row r="262" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>983</v>
       </c>
@@ -16596,7 +16627,7 @@
         <v>23</v>
       </c>
       <c r="J262" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="K262" t="s">
         <v>41</v>
@@ -16617,7 +16648,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="263" spans="1:16">
+    <row r="263" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>989</v>
       </c>
@@ -16646,7 +16677,7 @@
         <v>23</v>
       </c>
       <c r="J263" s="1">
-        <v>75.4</v>
+        <v>75.400000000000006</v>
       </c>
       <c r="K263" t="s">
         <v>24</v>
@@ -16667,7 +16698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="264" spans="1:16">
+    <row r="264" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>993</v>
       </c>
@@ -16717,7 +16748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="265" spans="1:16">
+    <row r="265" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>998</v>
       </c>
@@ -16767,7 +16798,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="266" spans="1:16">
+    <row r="266" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>1002</v>
       </c>
@@ -16796,7 +16827,7 @@
         <v>23</v>
       </c>
       <c r="J266" s="1">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="K266" t="s">
         <v>260</v>
@@ -16817,7 +16848,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="267" spans="1:16">
+    <row r="267" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>1002</v>
       </c>
@@ -16846,7 +16877,7 @@
         <v>23</v>
       </c>
       <c r="J267" s="1">
-        <v>184.0</v>
+        <v>184</v>
       </c>
       <c r="K267" t="s">
         <v>260</v>
@@ -16867,7 +16898,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="268" spans="1:16">
+    <row r="268" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>1002</v>
       </c>
@@ -16896,7 +16927,7 @@
         <v>23</v>
       </c>
       <c r="J268" s="1">
-        <v>95.0</v>
+        <v>95</v>
       </c>
       <c r="K268" t="s">
         <v>260</v>
@@ -16917,7 +16948,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="269" spans="1:16">
+    <row r="269" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>1012</v>
       </c>
@@ -16967,7 +16998,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="270" spans="1:16">
+    <row r="270" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>1016</v>
       </c>
@@ -17017,7 +17048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="271" spans="1:16">
+    <row r="271" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>1020</v>
       </c>
@@ -17067,7 +17098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="272" spans="1:16">
+    <row r="272" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>1024</v>
       </c>
@@ -17117,7 +17148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="273" spans="1:16">
+    <row r="273" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>1028</v>
       </c>
@@ -17167,7 +17198,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="274" spans="1:16">
+    <row r="274" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>1028</v>
       </c>
@@ -17196,7 +17227,7 @@
         <v>23</v>
       </c>
       <c r="J274" s="1">
-        <v>277.0</v>
+        <v>277</v>
       </c>
       <c r="K274" t="s">
         <v>41</v>
@@ -17217,7 +17248,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="275" spans="1:16">
+    <row r="275" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>1028</v>
       </c>
@@ -17246,7 +17277,7 @@
         <v>23</v>
       </c>
       <c r="J275" s="1">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="K275" t="s">
         <v>41</v>
@@ -17267,7 +17298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="276" spans="1:16">
+    <row r="276" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>1036</v>
       </c>
@@ -17296,7 +17327,7 @@
         <v>23</v>
       </c>
       <c r="J276" s="1">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="K276" t="s">
         <v>24</v>
@@ -17317,7 +17348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="277" spans="1:16">
+    <row r="277" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>1036</v>
       </c>
@@ -17346,7 +17377,7 @@
         <v>23</v>
       </c>
       <c r="J277" s="1">
-        <v>421.0</v>
+        <v>421</v>
       </c>
       <c r="K277" t="s">
         <v>41</v>
@@ -17367,7 +17398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="278" spans="1:16">
+    <row r="278" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>1036</v>
       </c>
@@ -17396,7 +17427,7 @@
         <v>23</v>
       </c>
       <c r="J278" s="1">
-        <v>677.0</v>
+        <v>677</v>
       </c>
       <c r="K278" t="s">
         <v>41</v>
@@ -17417,7 +17448,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="279" spans="1:16">
+    <row r="279" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>1044</v>
       </c>
@@ -17467,7 +17498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="280" spans="1:16">
+    <row r="280" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>1044</v>
       </c>
@@ -17517,7 +17548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="281" spans="1:16">
+    <row r="281" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>1048</v>
       </c>
@@ -17567,7 +17598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="282" spans="1:16">
+    <row r="282" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>1052</v>
       </c>
@@ -17596,7 +17627,7 @@
         <v>23</v>
       </c>
       <c r="J282" s="1">
-        <v>71.4</v>
+        <v>71.400000000000006</v>
       </c>
       <c r="K282" t="s">
         <v>24</v>
@@ -17618,17 +17649,13 @@
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <autoFilter ref="A1:P282" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="byt"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>